<commit_message>
Adicionada mostragem de resultados tamura
</commit_message>
<xml_diff>
--- a/rois_informations.xlsx
+++ b/rois_informations.xlsx
@@ -543,49 +543,61 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>299, 182</t>
+          <t>234, 204</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>236, 204</t>
+          <t>291, 177</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1.031408082717216</v>
+        <v>0.9960743658856868</v>
       </c>
       <c r="F2" t="n">
-        <v>11.1602473356761</v>
+        <v>11.25418873922899</v>
       </c>
       <c r="G2" t="n">
-        <v>11.1602473356761</v>
+        <v>11.25418873922899</v>
       </c>
       <c r="H2" t="n">
-        <v>11.31468450417742</v>
+        <v>11.48112966818735</v>
       </c>
       <c r="I2" t="n">
-        <v>11.31468450417742</v>
+        <v>11.48112966818735</v>
       </c>
       <c r="J2" t="n">
-        <v>11.32829441735521</v>
+        <v>11.53161503560841</v>
       </c>
       <c r="K2" t="n">
-        <v>11.32829441735521</v>
+        <v>11.53161503560841</v>
       </c>
       <c r="L2" t="n">
-        <v>11.24055642681196</v>
+        <v>11.48302527749911</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>11.240556426811963</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
+          <t>11.48302527749911</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>103.3054846938776</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.7622791325100794</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1166.640882837664</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.3931213017751479</v>
+      </c>
+      <c r="R2" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="S2" t="n">
+        <v>78.74761525598225</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">

</xml_diff>